<commit_message>
changes and more changes
</commit_message>
<xml_diff>
--- a/All Scrapped Excels/Combined id.xlsx
+++ b/All Scrapped Excels/Combined id.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D427"/>
+  <dimension ref="A1:E427"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>Product_id</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Price_id</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -463,6 +468,9 @@
       <c r="D2" t="n">
         <v>1</v>
       </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -477,6 +485,9 @@
       <c r="D3" t="n">
         <v>2</v>
       </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -491,6 +502,9 @@
       <c r="D4" t="n">
         <v>3</v>
       </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -503,6 +517,9 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
         <v>4</v>
       </c>
     </row>
@@ -519,6 +536,9 @@
       <c r="D6" t="n">
         <v>5</v>
       </c>
+      <c r="E6" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -533,6 +553,9 @@
       <c r="D7" t="n">
         <v>6</v>
       </c>
+      <c r="E7" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -547,6 +570,9 @@
       <c r="D8" t="n">
         <v>7</v>
       </c>
+      <c r="E8" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -561,6 +587,9 @@
       <c r="D9" t="n">
         <v>8</v>
       </c>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -575,6 +604,9 @@
       <c r="D10" t="n">
         <v>9</v>
       </c>
+      <c r="E10" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -589,6 +621,9 @@
       <c r="D11" t="n">
         <v>10</v>
       </c>
+      <c r="E11" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -603,6 +638,9 @@
       <c r="D12" t="n">
         <v>11</v>
       </c>
+      <c r="E12" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -617,6 +655,9 @@
       <c r="D13" t="n">
         <v>12</v>
       </c>
+      <c r="E13" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -631,6 +672,9 @@
       <c r="D14" t="n">
         <v>13</v>
       </c>
+      <c r="E14" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -645,6 +689,9 @@
       <c r="D15" t="n">
         <v>14</v>
       </c>
+      <c r="E15" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -659,6 +706,9 @@
       <c r="D16" t="n">
         <v>15</v>
       </c>
+      <c r="E16" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -673,6 +723,9 @@
       <c r="D17" t="n">
         <v>16</v>
       </c>
+      <c r="E17" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -687,6 +740,9 @@
       <c r="D18" t="n">
         <v>17</v>
       </c>
+      <c r="E18" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -701,6 +757,9 @@
       <c r="D19" t="n">
         <v>18</v>
       </c>
+      <c r="E19" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -715,6 +774,9 @@
       <c r="D20" t="n">
         <v>19</v>
       </c>
+      <c r="E20" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -729,6 +791,9 @@
       <c r="D21" t="n">
         <v>20</v>
       </c>
+      <c r="E21" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -743,6 +808,9 @@
       <c r="D22" t="n">
         <v>21</v>
       </c>
+      <c r="E22" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -757,6 +825,9 @@
       <c r="D23" t="n">
         <v>22</v>
       </c>
+      <c r="E23" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -771,6 +842,9 @@
       <c r="D24" t="n">
         <v>23</v>
       </c>
+      <c r="E24" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -785,6 +859,9 @@
       <c r="D25" t="n">
         <v>24</v>
       </c>
+      <c r="E25" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -799,6 +876,9 @@
       <c r="D26" t="n">
         <v>25</v>
       </c>
+      <c r="E26" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -813,6 +893,9 @@
       <c r="D27" t="n">
         <v>26</v>
       </c>
+      <c r="E27" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -827,6 +910,9 @@
       <c r="D28" t="n">
         <v>27</v>
       </c>
+      <c r="E28" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -841,6 +927,9 @@
       <c r="D29" t="n">
         <v>28</v>
       </c>
+      <c r="E29" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -855,6 +944,9 @@
       <c r="D30" t="n">
         <v>29</v>
       </c>
+      <c r="E30" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -869,6 +961,9 @@
       <c r="D31" t="n">
         <v>30</v>
       </c>
+      <c r="E31" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -883,6 +978,9 @@
       <c r="D32" t="n">
         <v>31</v>
       </c>
+      <c r="E32" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -897,6 +995,9 @@
       <c r="D33" t="n">
         <v>32</v>
       </c>
+      <c r="E33" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -911,6 +1012,9 @@
       <c r="D34" t="n">
         <v>33</v>
       </c>
+      <c r="E34" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -925,6 +1029,9 @@
       <c r="D35" t="n">
         <v>34</v>
       </c>
+      <c r="E35" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -939,6 +1046,9 @@
       <c r="D36" t="n">
         <v>35</v>
       </c>
+      <c r="E36" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -953,6 +1063,9 @@
       <c r="D37" t="n">
         <v>36</v>
       </c>
+      <c r="E37" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -967,6 +1080,9 @@
       <c r="D38" t="n">
         <v>37</v>
       </c>
+      <c r="E38" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -981,6 +1097,9 @@
       <c r="D39" t="n">
         <v>38</v>
       </c>
+      <c r="E39" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -995,6 +1114,9 @@
       <c r="D40" t="n">
         <v>39</v>
       </c>
+      <c r="E40" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1009,6 +1131,9 @@
       <c r="D41" t="n">
         <v>40</v>
       </c>
+      <c r="E41" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1023,6 +1148,9 @@
       <c r="D42" t="n">
         <v>41</v>
       </c>
+      <c r="E42" t="n">
+        <v>41</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1037,6 +1165,9 @@
       <c r="D43" t="n">
         <v>42</v>
       </c>
+      <c r="E43" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1051,6 +1182,9 @@
       <c r="D44" t="n">
         <v>43</v>
       </c>
+      <c r="E44" t="n">
+        <v>43</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1065,6 +1199,9 @@
       <c r="D45" t="n">
         <v>44</v>
       </c>
+      <c r="E45" t="n">
+        <v>44</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1079,6 +1216,9 @@
       <c r="D46" t="n">
         <v>45</v>
       </c>
+      <c r="E46" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1093,6 +1233,9 @@
       <c r="D47" t="n">
         <v>46</v>
       </c>
+      <c r="E47" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1107,6 +1250,9 @@
       <c r="D48" t="n">
         <v>47</v>
       </c>
+      <c r="E48" t="n">
+        <v>47</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1121,6 +1267,9 @@
       <c r="D49" t="n">
         <v>48</v>
       </c>
+      <c r="E49" t="n">
+        <v>48</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1135,6 +1284,9 @@
       <c r="D50" t="n">
         <v>49</v>
       </c>
+      <c r="E50" t="n">
+        <v>49</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1149,6 +1301,9 @@
       <c r="D51" t="n">
         <v>50</v>
       </c>
+      <c r="E51" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1163,6 +1318,9 @@
       <c r="D52" t="n">
         <v>51</v>
       </c>
+      <c r="E52" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1177,6 +1335,9 @@
       <c r="D53" t="n">
         <v>52</v>
       </c>
+      <c r="E53" t="n">
+        <v>52</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1191,6 +1352,9 @@
       <c r="D54" t="n">
         <v>53</v>
       </c>
+      <c r="E54" t="n">
+        <v>53</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1205,6 +1369,9 @@
       <c r="D55" t="n">
         <v>54</v>
       </c>
+      <c r="E55" t="n">
+        <v>54</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -1219,6 +1386,9 @@
       <c r="D56" t="n">
         <v>55</v>
       </c>
+      <c r="E56" t="n">
+        <v>55</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -1233,6 +1403,9 @@
       <c r="D57" t="n">
         <v>56</v>
       </c>
+      <c r="E57" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1247,6 +1420,9 @@
       <c r="D58" t="n">
         <v>57</v>
       </c>
+      <c r="E58" t="n">
+        <v>57</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -1261,6 +1437,9 @@
       <c r="D59" t="n">
         <v>58</v>
       </c>
+      <c r="E59" t="n">
+        <v>58</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -1275,6 +1454,9 @@
       <c r="D60" t="n">
         <v>59</v>
       </c>
+      <c r="E60" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -1289,6 +1471,9 @@
       <c r="D61" t="n">
         <v>60</v>
       </c>
+      <c r="E61" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -1303,6 +1488,9 @@
       <c r="D62" t="n">
         <v>61</v>
       </c>
+      <c r="E62" t="n">
+        <v>61</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -1317,6 +1505,9 @@
       <c r="D63" t="n">
         <v>62</v>
       </c>
+      <c r="E63" t="n">
+        <v>62</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -1331,6 +1522,9 @@
       <c r="D64" t="n">
         <v>63</v>
       </c>
+      <c r="E64" t="n">
+        <v>63</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -1345,6 +1539,9 @@
       <c r="D65" t="n">
         <v>64</v>
       </c>
+      <c r="E65" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -1359,6 +1556,9 @@
       <c r="D66" t="n">
         <v>65</v>
       </c>
+      <c r="E66" t="n">
+        <v>65</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -1373,6 +1573,9 @@
       <c r="D67" t="n">
         <v>66</v>
       </c>
+      <c r="E67" t="n">
+        <v>66</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -1387,6 +1590,9 @@
       <c r="D68" t="n">
         <v>67</v>
       </c>
+      <c r="E68" t="n">
+        <v>67</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -1401,6 +1607,9 @@
       <c r="D69" t="n">
         <v>68</v>
       </c>
+      <c r="E69" t="n">
+        <v>68</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -1415,6 +1624,9 @@
       <c r="D70" t="n">
         <v>69</v>
       </c>
+      <c r="E70" t="n">
+        <v>69</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -1429,6 +1641,9 @@
       <c r="D71" t="n">
         <v>70</v>
       </c>
+      <c r="E71" t="n">
+        <v>70</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -1443,6 +1658,9 @@
       <c r="D72" t="n">
         <v>71</v>
       </c>
+      <c r="E72" t="n">
+        <v>71</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -1457,6 +1675,9 @@
       <c r="D73" t="n">
         <v>72</v>
       </c>
+      <c r="E73" t="n">
+        <v>72</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -1471,6 +1692,9 @@
       <c r="D74" t="n">
         <v>73</v>
       </c>
+      <c r="E74" t="n">
+        <v>73</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -1485,6 +1709,9 @@
       <c r="D75" t="n">
         <v>74</v>
       </c>
+      <c r="E75" t="n">
+        <v>74</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -1499,6 +1726,9 @@
       <c r="D76" t="n">
         <v>75</v>
       </c>
+      <c r="E76" t="n">
+        <v>75</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -1513,6 +1743,9 @@
       <c r="D77" t="n">
         <v>76</v>
       </c>
+      <c r="E77" t="n">
+        <v>76</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -1527,6 +1760,9 @@
       <c r="D78" t="n">
         <v>77</v>
       </c>
+      <c r="E78" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -1541,6 +1777,9 @@
       <c r="D79" t="n">
         <v>78</v>
       </c>
+      <c r="E79" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -1555,6 +1794,9 @@
       <c r="D80" t="n">
         <v>79</v>
       </c>
+      <c r="E80" t="n">
+        <v>79</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -1569,6 +1811,9 @@
       <c r="D81" t="n">
         <v>80</v>
       </c>
+      <c r="E81" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -1583,6 +1828,9 @@
       <c r="D82" t="n">
         <v>81</v>
       </c>
+      <c r="E82" t="n">
+        <v>81</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -1597,6 +1845,9 @@
       <c r="D83" t="n">
         <v>82</v>
       </c>
+      <c r="E83" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -1611,6 +1862,9 @@
       <c r="D84" t="n">
         <v>83</v>
       </c>
+      <c r="E84" t="n">
+        <v>83</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -1625,6 +1879,9 @@
       <c r="D85" t="n">
         <v>84</v>
       </c>
+      <c r="E85" t="n">
+        <v>84</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -1639,6 +1896,9 @@
       <c r="D86" t="n">
         <v>85</v>
       </c>
+      <c r="E86" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -1653,6 +1913,9 @@
       <c r="D87" t="n">
         <v>86</v>
       </c>
+      <c r="E87" t="n">
+        <v>86</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -1667,6 +1930,9 @@
       <c r="D88" t="n">
         <v>87</v>
       </c>
+      <c r="E88" t="n">
+        <v>87</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -1681,6 +1947,9 @@
       <c r="D89" t="n">
         <v>88</v>
       </c>
+      <c r="E89" t="n">
+        <v>88</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -1695,6 +1964,9 @@
       <c r="D90" t="n">
         <v>89</v>
       </c>
+      <c r="E90" t="n">
+        <v>89</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -1709,6 +1981,9 @@
       <c r="D91" t="n">
         <v>90</v>
       </c>
+      <c r="E91" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -1723,6 +1998,9 @@
       <c r="D92" t="n">
         <v>91</v>
       </c>
+      <c r="E92" t="n">
+        <v>91</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -1737,6 +2015,9 @@
       <c r="D93" t="n">
         <v>92</v>
       </c>
+      <c r="E93" t="n">
+        <v>92</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -1751,6 +2032,9 @@
       <c r="D94" t="n">
         <v>93</v>
       </c>
+      <c r="E94" t="n">
+        <v>93</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -1765,6 +2049,9 @@
       <c r="D95" t="n">
         <v>94</v>
       </c>
+      <c r="E95" t="n">
+        <v>94</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -1779,6 +2066,9 @@
       <c r="D96" t="n">
         <v>95</v>
       </c>
+      <c r="E96" t="n">
+        <v>95</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -1793,6 +2083,9 @@
       <c r="D97" t="n">
         <v>96</v>
       </c>
+      <c r="E97" t="n">
+        <v>96</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -1807,6 +2100,9 @@
       <c r="D98" t="n">
         <v>97</v>
       </c>
+      <c r="E98" t="n">
+        <v>97</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -1821,6 +2117,9 @@
       <c r="D99" t="n">
         <v>98</v>
       </c>
+      <c r="E99" t="n">
+        <v>98</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -1835,6 +2134,9 @@
       <c r="D100" t="n">
         <v>99</v>
       </c>
+      <c r="E100" t="n">
+        <v>99</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -1849,6 +2151,9 @@
       <c r="D101" t="n">
         <v>100</v>
       </c>
+      <c r="E101" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -1863,6 +2168,9 @@
       <c r="D102" t="n">
         <v>101</v>
       </c>
+      <c r="E102" t="n">
+        <v>101</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -1877,6 +2185,9 @@
       <c r="D103" t="n">
         <v>102</v>
       </c>
+      <c r="E103" t="n">
+        <v>102</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -1891,6 +2202,9 @@
       <c r="D104" t="n">
         <v>103</v>
       </c>
+      <c r="E104" t="n">
+        <v>103</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -1905,6 +2219,9 @@
       <c r="D105" t="n">
         <v>104</v>
       </c>
+      <c r="E105" t="n">
+        <v>104</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -1919,6 +2236,9 @@
       <c r="D106" t="n">
         <v>105</v>
       </c>
+      <c r="E106" t="n">
+        <v>105</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -1933,6 +2253,9 @@
       <c r="D107" t="n">
         <v>106</v>
       </c>
+      <c r="E107" t="n">
+        <v>106</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -1947,6 +2270,9 @@
       <c r="D108" t="n">
         <v>107</v>
       </c>
+      <c r="E108" t="n">
+        <v>107</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -1961,6 +2287,9 @@
       <c r="D109" t="n">
         <v>108</v>
       </c>
+      <c r="E109" t="n">
+        <v>108</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -1975,6 +2304,9 @@
       <c r="D110" t="n">
         <v>109</v>
       </c>
+      <c r="E110" t="n">
+        <v>109</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -1989,6 +2321,9 @@
       <c r="D111" t="n">
         <v>110</v>
       </c>
+      <c r="E111" t="n">
+        <v>110</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -2003,6 +2338,9 @@
       <c r="D112" t="n">
         <v>111</v>
       </c>
+      <c r="E112" t="n">
+        <v>111</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -2017,6 +2355,9 @@
       <c r="D113" t="n">
         <v>112</v>
       </c>
+      <c r="E113" t="n">
+        <v>112</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -2031,6 +2372,9 @@
       <c r="D114" t="n">
         <v>113</v>
       </c>
+      <c r="E114" t="n">
+        <v>113</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -2045,6 +2389,9 @@
       <c r="D115" t="n">
         <v>114</v>
       </c>
+      <c r="E115" t="n">
+        <v>114</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -2059,6 +2406,9 @@
       <c r="D116" t="n">
         <v>115</v>
       </c>
+      <c r="E116" t="n">
+        <v>115</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -2073,6 +2423,9 @@
       <c r="D117" t="n">
         <v>116</v>
       </c>
+      <c r="E117" t="n">
+        <v>116</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -2087,6 +2440,9 @@
       <c r="D118" t="n">
         <v>117</v>
       </c>
+      <c r="E118" t="n">
+        <v>117</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -2101,6 +2457,9 @@
       <c r="D119" t="n">
         <v>118</v>
       </c>
+      <c r="E119" t="n">
+        <v>118</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -2115,6 +2474,9 @@
       <c r="D120" t="n">
         <v>119</v>
       </c>
+      <c r="E120" t="n">
+        <v>119</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -2129,6 +2491,9 @@
       <c r="D121" t="n">
         <v>120</v>
       </c>
+      <c r="E121" t="n">
+        <v>120</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -2143,6 +2508,9 @@
       <c r="D122" t="n">
         <v>121</v>
       </c>
+      <c r="E122" t="n">
+        <v>121</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -2157,6 +2525,9 @@
       <c r="D123" t="n">
         <v>122</v>
       </c>
+      <c r="E123" t="n">
+        <v>122</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -2171,6 +2542,9 @@
       <c r="D124" t="n">
         <v>123</v>
       </c>
+      <c r="E124" t="n">
+        <v>123</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -2185,6 +2559,9 @@
       <c r="D125" t="n">
         <v>124</v>
       </c>
+      <c r="E125" t="n">
+        <v>124</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -2199,6 +2576,9 @@
       <c r="D126" t="n">
         <v>125</v>
       </c>
+      <c r="E126" t="n">
+        <v>125</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -2213,6 +2593,9 @@
       <c r="D127" t="n">
         <v>126</v>
       </c>
+      <c r="E127" t="n">
+        <v>126</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -2227,6 +2610,9 @@
       <c r="D128" t="n">
         <v>127</v>
       </c>
+      <c r="E128" t="n">
+        <v>127</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -2241,6 +2627,9 @@
       <c r="D129" t="n">
         <v>128</v>
       </c>
+      <c r="E129" t="n">
+        <v>128</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -2255,6 +2644,9 @@
       <c r="D130" t="n">
         <v>129</v>
       </c>
+      <c r="E130" t="n">
+        <v>129</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -2269,6 +2661,9 @@
       <c r="D131" t="n">
         <v>130</v>
       </c>
+      <c r="E131" t="n">
+        <v>130</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -2283,6 +2678,9 @@
       <c r="D132" t="n">
         <v>131</v>
       </c>
+      <c r="E132" t="n">
+        <v>131</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -2297,6 +2695,9 @@
       <c r="D133" t="n">
         <v>132</v>
       </c>
+      <c r="E133" t="n">
+        <v>132</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -2311,6 +2712,9 @@
       <c r="D134" t="n">
         <v>133</v>
       </c>
+      <c r="E134" t="n">
+        <v>133</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -2325,6 +2729,9 @@
       <c r="D135" t="n">
         <v>134</v>
       </c>
+      <c r="E135" t="n">
+        <v>134</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -2339,6 +2746,9 @@
       <c r="D136" t="n">
         <v>135</v>
       </c>
+      <c r="E136" t="n">
+        <v>135</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -2353,6 +2763,9 @@
       <c r="D137" t="n">
         <v>136</v>
       </c>
+      <c r="E137" t="n">
+        <v>136</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -2367,6 +2780,9 @@
       <c r="D138" t="n">
         <v>137</v>
       </c>
+      <c r="E138" t="n">
+        <v>137</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -2381,6 +2797,9 @@
       <c r="D139" t="n">
         <v>138</v>
       </c>
+      <c r="E139" t="n">
+        <v>138</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -2395,6 +2814,9 @@
       <c r="D140" t="n">
         <v>139</v>
       </c>
+      <c r="E140" t="n">
+        <v>139</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -2409,6 +2831,9 @@
       <c r="D141" t="n">
         <v>140</v>
       </c>
+      <c r="E141" t="n">
+        <v>140</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -2423,6 +2848,9 @@
       <c r="D142" t="n">
         <v>141</v>
       </c>
+      <c r="E142" t="n">
+        <v>141</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -2437,6 +2865,9 @@
       <c r="D143" t="n">
         <v>142</v>
       </c>
+      <c r="E143" t="n">
+        <v>142</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -2451,6 +2882,9 @@
       <c r="D144" t="n">
         <v>143</v>
       </c>
+      <c r="E144" t="n">
+        <v>143</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -2465,6 +2899,9 @@
       <c r="D145" t="n">
         <v>144</v>
       </c>
+      <c r="E145" t="n">
+        <v>144</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -2479,6 +2916,9 @@
       <c r="D146" t="n">
         <v>145</v>
       </c>
+      <c r="E146" t="n">
+        <v>145</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -2493,6 +2933,9 @@
       <c r="D147" t="n">
         <v>146</v>
       </c>
+      <c r="E147" t="n">
+        <v>146</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -2507,6 +2950,9 @@
       <c r="D148" t="n">
         <v>147</v>
       </c>
+      <c r="E148" t="n">
+        <v>147</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -2521,6 +2967,9 @@
       <c r="D149" t="n">
         <v>148</v>
       </c>
+      <c r="E149" t="n">
+        <v>148</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -2535,6 +2984,9 @@
       <c r="D150" t="n">
         <v>149</v>
       </c>
+      <c r="E150" t="n">
+        <v>149</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -2549,6 +3001,9 @@
       <c r="D151" t="n">
         <v>150</v>
       </c>
+      <c r="E151" t="n">
+        <v>150</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -2563,6 +3018,9 @@
       <c r="D152" t="n">
         <v>151</v>
       </c>
+      <c r="E152" t="n">
+        <v>151</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -2577,6 +3035,9 @@
       <c r="D153" t="n">
         <v>152</v>
       </c>
+      <c r="E153" t="n">
+        <v>152</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -2591,6 +3052,9 @@
       <c r="D154" t="n">
         <v>153</v>
       </c>
+      <c r="E154" t="n">
+        <v>153</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -2605,6 +3069,9 @@
       <c r="D155" t="n">
         <v>154</v>
       </c>
+      <c r="E155" t="n">
+        <v>154</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -2619,6 +3086,9 @@
       <c r="D156" t="n">
         <v>155</v>
       </c>
+      <c r="E156" t="n">
+        <v>155</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -2633,6 +3103,9 @@
       <c r="D157" t="n">
         <v>156</v>
       </c>
+      <c r="E157" t="n">
+        <v>156</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -2647,6 +3120,9 @@
       <c r="D158" t="n">
         <v>157</v>
       </c>
+      <c r="E158" t="n">
+        <v>157</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -2661,6 +3137,9 @@
       <c r="D159" t="n">
         <v>158</v>
       </c>
+      <c r="E159" t="n">
+        <v>158</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -2675,6 +3154,9 @@
       <c r="D160" t="n">
         <v>159</v>
       </c>
+      <c r="E160" t="n">
+        <v>159</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -2689,6 +3171,9 @@
       <c r="D161" t="n">
         <v>160</v>
       </c>
+      <c r="E161" t="n">
+        <v>160</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -2703,6 +3188,9 @@
       <c r="D162" t="n">
         <v>161</v>
       </c>
+      <c r="E162" t="n">
+        <v>161</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -2717,6 +3205,9 @@
       <c r="D163" t="n">
         <v>162</v>
       </c>
+      <c r="E163" t="n">
+        <v>162</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -2731,6 +3222,9 @@
       <c r="D164" t="n">
         <v>163</v>
       </c>
+      <c r="E164" t="n">
+        <v>163</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -2745,6 +3239,9 @@
       <c r="D165" t="n">
         <v>164</v>
       </c>
+      <c r="E165" t="n">
+        <v>164</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -2759,6 +3256,9 @@
       <c r="D166" t="n">
         <v>165</v>
       </c>
+      <c r="E166" t="n">
+        <v>165</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -2773,6 +3273,9 @@
       <c r="D167" t="n">
         <v>166</v>
       </c>
+      <c r="E167" t="n">
+        <v>166</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -2787,6 +3290,9 @@
       <c r="D168" t="n">
         <v>167</v>
       </c>
+      <c r="E168" t="n">
+        <v>167</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -2801,6 +3307,9 @@
       <c r="D169" t="n">
         <v>168</v>
       </c>
+      <c r="E169" t="n">
+        <v>168</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -2815,6 +3324,9 @@
       <c r="D170" t="n">
         <v>169</v>
       </c>
+      <c r="E170" t="n">
+        <v>169</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -2829,6 +3341,9 @@
       <c r="D171" t="n">
         <v>170</v>
       </c>
+      <c r="E171" t="n">
+        <v>170</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
@@ -2843,6 +3358,9 @@
       <c r="D172" t="n">
         <v>171</v>
       </c>
+      <c r="E172" t="n">
+        <v>171</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
@@ -2857,6 +3375,9 @@
       <c r="D173" t="n">
         <v>172</v>
       </c>
+      <c r="E173" t="n">
+        <v>172</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -2871,6 +3392,9 @@
       <c r="D174" t="n">
         <v>173</v>
       </c>
+      <c r="E174" t="n">
+        <v>173</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
@@ -2885,6 +3409,9 @@
       <c r="D175" t="n">
         <v>174</v>
       </c>
+      <c r="E175" t="n">
+        <v>174</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -2899,6 +3426,9 @@
       <c r="D176" t="n">
         <v>175</v>
       </c>
+      <c r="E176" t="n">
+        <v>175</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -2913,6 +3443,9 @@
       <c r="D177" t="n">
         <v>176</v>
       </c>
+      <c r="E177" t="n">
+        <v>176</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
@@ -2927,6 +3460,9 @@
       <c r="D178" t="n">
         <v>177</v>
       </c>
+      <c r="E178" t="n">
+        <v>177</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -2941,6 +3477,9 @@
       <c r="D179" t="n">
         <v>178</v>
       </c>
+      <c r="E179" t="n">
+        <v>178</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -2955,6 +3494,9 @@
       <c r="D180" t="n">
         <v>179</v>
       </c>
+      <c r="E180" t="n">
+        <v>179</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -2969,6 +3511,9 @@
       <c r="D181" t="n">
         <v>180</v>
       </c>
+      <c r="E181" t="n">
+        <v>180</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
@@ -2983,6 +3528,9 @@
       <c r="D182" t="n">
         <v>181</v>
       </c>
+      <c r="E182" t="n">
+        <v>181</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -2997,6 +3545,9 @@
       <c r="D183" t="n">
         <v>182</v>
       </c>
+      <c r="E183" t="n">
+        <v>182</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -3011,6 +3562,9 @@
       <c r="D184" t="n">
         <v>183</v>
       </c>
+      <c r="E184" t="n">
+        <v>183</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -3025,6 +3579,9 @@
       <c r="D185" t="n">
         <v>184</v>
       </c>
+      <c r="E185" t="n">
+        <v>184</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
@@ -3039,6 +3596,9 @@
       <c r="D186" t="n">
         <v>185</v>
       </c>
+      <c r="E186" t="n">
+        <v>185</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -3053,6 +3613,9 @@
       <c r="D187" t="n">
         <v>186</v>
       </c>
+      <c r="E187" t="n">
+        <v>186</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
@@ -3067,6 +3630,9 @@
       <c r="D188" t="n">
         <v>187</v>
       </c>
+      <c r="E188" t="n">
+        <v>187</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -3081,6 +3647,9 @@
       <c r="D189" t="n">
         <v>188</v>
       </c>
+      <c r="E189" t="n">
+        <v>188</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -3095,6 +3664,9 @@
       <c r="D190" t="n">
         <v>189</v>
       </c>
+      <c r="E190" t="n">
+        <v>189</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
@@ -3109,6 +3681,9 @@
       <c r="D191" t="n">
         <v>190</v>
       </c>
+      <c r="E191" t="n">
+        <v>190</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
@@ -3123,6 +3698,9 @@
       <c r="D192" t="n">
         <v>191</v>
       </c>
+      <c r="E192" t="n">
+        <v>191</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -3137,6 +3715,9 @@
       <c r="D193" t="n">
         <v>192</v>
       </c>
+      <c r="E193" t="n">
+        <v>192</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
@@ -3151,6 +3732,9 @@
       <c r="D194" t="n">
         <v>193</v>
       </c>
+      <c r="E194" t="n">
+        <v>193</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
@@ -3165,6 +3749,9 @@
       <c r="D195" t="n">
         <v>194</v>
       </c>
+      <c r="E195" t="n">
+        <v>194</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -3179,6 +3766,9 @@
       <c r="D196" t="n">
         <v>195</v>
       </c>
+      <c r="E196" t="n">
+        <v>195</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
@@ -3193,6 +3783,9 @@
       <c r="D197" t="n">
         <v>196</v>
       </c>
+      <c r="E197" t="n">
+        <v>196</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -3207,6 +3800,9 @@
       <c r="D198" t="n">
         <v>197</v>
       </c>
+      <c r="E198" t="n">
+        <v>197</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
@@ -3221,6 +3817,9 @@
       <c r="D199" t="n">
         <v>198</v>
       </c>
+      <c r="E199" t="n">
+        <v>198</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
@@ -3235,6 +3834,9 @@
       <c r="D200" t="n">
         <v>199</v>
       </c>
+      <c r="E200" t="n">
+        <v>199</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -3249,6 +3851,9 @@
       <c r="D201" t="n">
         <v>200</v>
       </c>
+      <c r="E201" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -3263,6 +3868,9 @@
       <c r="D202" t="n">
         <v>201</v>
       </c>
+      <c r="E202" t="n">
+        <v>201</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
@@ -3277,6 +3885,9 @@
       <c r="D203" t="n">
         <v>202</v>
       </c>
+      <c r="E203" t="n">
+        <v>202</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
@@ -3291,6 +3902,9 @@
       <c r="D204" t="n">
         <v>203</v>
       </c>
+      <c r="E204" t="n">
+        <v>203</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
@@ -3305,6 +3919,9 @@
       <c r="D205" t="n">
         <v>204</v>
       </c>
+      <c r="E205" t="n">
+        <v>204</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
@@ -3319,6 +3936,9 @@
       <c r="D206" t="n">
         <v>205</v>
       </c>
+      <c r="E206" t="n">
+        <v>205</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
@@ -3333,6 +3953,9 @@
       <c r="D207" t="n">
         <v>206</v>
       </c>
+      <c r="E207" t="n">
+        <v>206</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
@@ -3347,6 +3970,9 @@
       <c r="D208" t="n">
         <v>207</v>
       </c>
+      <c r="E208" t="n">
+        <v>207</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
@@ -3361,6 +3987,9 @@
       <c r="D209" t="n">
         <v>208</v>
       </c>
+      <c r="E209" t="n">
+        <v>208</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -3375,6 +4004,9 @@
       <c r="D210" t="n">
         <v>209</v>
       </c>
+      <c r="E210" t="n">
+        <v>209</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
@@ -3389,6 +4021,9 @@
       <c r="D211" t="n">
         <v>210</v>
       </c>
+      <c r="E211" t="n">
+        <v>210</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
@@ -3403,6 +4038,9 @@
       <c r="D212" t="n">
         <v>211</v>
       </c>
+      <c r="E212" t="n">
+        <v>211</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
@@ -3417,6 +4055,9 @@
       <c r="D213" t="n">
         <v>212</v>
       </c>
+      <c r="E213" t="n">
+        <v>212</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
@@ -3431,6 +4072,9 @@
       <c r="D214" t="n">
         <v>213</v>
       </c>
+      <c r="E214" t="n">
+        <v>213</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
@@ -3445,6 +4089,9 @@
       <c r="D215" t="n">
         <v>214</v>
       </c>
+      <c r="E215" t="n">
+        <v>214</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
@@ -3459,6 +4106,9 @@
       <c r="D216" t="n">
         <v>215</v>
       </c>
+      <c r="E216" t="n">
+        <v>215</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -3473,6 +4123,9 @@
       <c r="D217" t="n">
         <v>216</v>
       </c>
+      <c r="E217" t="n">
+        <v>216</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
@@ -3487,6 +4140,9 @@
       <c r="D218" t="n">
         <v>217</v>
       </c>
+      <c r="E218" t="n">
+        <v>217</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
@@ -3501,6 +4157,9 @@
       <c r="D219" t="n">
         <v>218</v>
       </c>
+      <c r="E219" t="n">
+        <v>218</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -3515,6 +4174,9 @@
       <c r="D220" t="n">
         <v>219</v>
       </c>
+      <c r="E220" t="n">
+        <v>219</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
@@ -3529,6 +4191,9 @@
       <c r="D221" t="n">
         <v>220</v>
       </c>
+      <c r="E221" t="n">
+        <v>220</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
@@ -3543,6 +4208,9 @@
       <c r="D222" t="n">
         <v>221</v>
       </c>
+      <c r="E222" t="n">
+        <v>221</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
@@ -3557,6 +4225,9 @@
       <c r="D223" t="n">
         <v>222</v>
       </c>
+      <c r="E223" t="n">
+        <v>222</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
@@ -3571,6 +4242,9 @@
       <c r="D224" t="n">
         <v>223</v>
       </c>
+      <c r="E224" t="n">
+        <v>223</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
@@ -3585,6 +4259,9 @@
       <c r="D225" t="n">
         <v>224</v>
       </c>
+      <c r="E225" t="n">
+        <v>224</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
@@ -3599,6 +4276,9 @@
       <c r="D226" t="n">
         <v>225</v>
       </c>
+      <c r="E226" t="n">
+        <v>225</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
@@ -3613,6 +4293,9 @@
       <c r="D227" t="n">
         <v>226</v>
       </c>
+      <c r="E227" t="n">
+        <v>226</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
@@ -3627,6 +4310,9 @@
       <c r="D228" t="n">
         <v>227</v>
       </c>
+      <c r="E228" t="n">
+        <v>227</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
@@ -3641,6 +4327,9 @@
       <c r="D229" t="n">
         <v>228</v>
       </c>
+      <c r="E229" t="n">
+        <v>228</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
@@ -3655,6 +4344,9 @@
       <c r="D230" t="n">
         <v>229</v>
       </c>
+      <c r="E230" t="n">
+        <v>229</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
@@ -3669,6 +4361,9 @@
       <c r="D231" t="n">
         <v>230</v>
       </c>
+      <c r="E231" t="n">
+        <v>230</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
@@ -3683,6 +4378,9 @@
       <c r="D232" t="n">
         <v>231</v>
       </c>
+      <c r="E232" t="n">
+        <v>231</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
@@ -3697,6 +4395,9 @@
       <c r="D233" t="n">
         <v>232</v>
       </c>
+      <c r="E233" t="n">
+        <v>232</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
@@ -3711,6 +4412,9 @@
       <c r="D234" t="n">
         <v>233</v>
       </c>
+      <c r="E234" t="n">
+        <v>233</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
@@ -3725,6 +4429,9 @@
       <c r="D235" t="n">
         <v>234</v>
       </c>
+      <c r="E235" t="n">
+        <v>234</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
@@ -3739,6 +4446,9 @@
       <c r="D236" t="n">
         <v>235</v>
       </c>
+      <c r="E236" t="n">
+        <v>235</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
@@ -3753,6 +4463,9 @@
       <c r="D237" t="n">
         <v>236</v>
       </c>
+      <c r="E237" t="n">
+        <v>236</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
@@ -3767,6 +4480,9 @@
       <c r="D238" t="n">
         <v>237</v>
       </c>
+      <c r="E238" t="n">
+        <v>237</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
@@ -3781,6 +4497,9 @@
       <c r="D239" t="n">
         <v>238</v>
       </c>
+      <c r="E239" t="n">
+        <v>238</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
@@ -3795,6 +4514,9 @@
       <c r="D240" t="n">
         <v>239</v>
       </c>
+      <c r="E240" t="n">
+        <v>239</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
@@ -3809,6 +4531,9 @@
       <c r="D241" t="n">
         <v>240</v>
       </c>
+      <c r="E241" t="n">
+        <v>240</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
@@ -3823,6 +4548,9 @@
       <c r="D242" t="n">
         <v>241</v>
       </c>
+      <c r="E242" t="n">
+        <v>241</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
@@ -3837,6 +4565,9 @@
       <c r="D243" t="n">
         <v>242</v>
       </c>
+      <c r="E243" t="n">
+        <v>242</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
@@ -3851,6 +4582,9 @@
       <c r="D244" t="n">
         <v>243</v>
       </c>
+      <c r="E244" t="n">
+        <v>243</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
@@ -3865,6 +4599,9 @@
       <c r="D245" t="n">
         <v>244</v>
       </c>
+      <c r="E245" t="n">
+        <v>244</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
@@ -3879,6 +4616,9 @@
       <c r="D246" t="n">
         <v>245</v>
       </c>
+      <c r="E246" t="n">
+        <v>245</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
@@ -3893,6 +4633,9 @@
       <c r="D247" t="n">
         <v>246</v>
       </c>
+      <c r="E247" t="n">
+        <v>246</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
@@ -3907,6 +4650,9 @@
       <c r="D248" t="n">
         <v>247</v>
       </c>
+      <c r="E248" t="n">
+        <v>247</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
@@ -3921,6 +4667,9 @@
       <c r="D249" t="n">
         <v>248</v>
       </c>
+      <c r="E249" t="n">
+        <v>248</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
@@ -3935,6 +4684,9 @@
       <c r="D250" t="n">
         <v>249</v>
       </c>
+      <c r="E250" t="n">
+        <v>249</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
@@ -3949,6 +4701,9 @@
       <c r="D251" t="n">
         <v>250</v>
       </c>
+      <c r="E251" t="n">
+        <v>250</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
@@ -3963,6 +4718,9 @@
       <c r="D252" t="n">
         <v>251</v>
       </c>
+      <c r="E252" t="n">
+        <v>251</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
@@ -3977,6 +4735,9 @@
       <c r="D253" t="n">
         <v>252</v>
       </c>
+      <c r="E253" t="n">
+        <v>252</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
@@ -3991,6 +4752,9 @@
       <c r="D254" t="n">
         <v>253</v>
       </c>
+      <c r="E254" t="n">
+        <v>253</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
@@ -4005,6 +4769,9 @@
       <c r="D255" t="n">
         <v>254</v>
       </c>
+      <c r="E255" t="n">
+        <v>254</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
@@ -4019,6 +4786,9 @@
       <c r="D256" t="n">
         <v>255</v>
       </c>
+      <c r="E256" t="n">
+        <v>255</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
@@ -4033,6 +4803,9 @@
       <c r="D257" t="n">
         <v>256</v>
       </c>
+      <c r="E257" t="n">
+        <v>256</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
@@ -4047,6 +4820,9 @@
       <c r="D258" t="n">
         <v>257</v>
       </c>
+      <c r="E258" t="n">
+        <v>257</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
@@ -4061,6 +4837,9 @@
       <c r="D259" t="n">
         <v>258</v>
       </c>
+      <c r="E259" t="n">
+        <v>258</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
@@ -4075,6 +4854,9 @@
       <c r="D260" t="n">
         <v>259</v>
       </c>
+      <c r="E260" t="n">
+        <v>259</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
@@ -4089,6 +4871,9 @@
       <c r="D261" t="n">
         <v>260</v>
       </c>
+      <c r="E261" t="n">
+        <v>260</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
@@ -4103,6 +4888,9 @@
       <c r="D262" t="n">
         <v>261</v>
       </c>
+      <c r="E262" t="n">
+        <v>261</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
@@ -4117,6 +4905,9 @@
       <c r="D263" t="n">
         <v>262</v>
       </c>
+      <c r="E263" t="n">
+        <v>262</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
@@ -4131,6 +4922,9 @@
       <c r="D264" t="n">
         <v>263</v>
       </c>
+      <c r="E264" t="n">
+        <v>263</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
@@ -4145,6 +4939,9 @@
       <c r="D265" t="n">
         <v>264</v>
       </c>
+      <c r="E265" t="n">
+        <v>264</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
@@ -4159,6 +4956,9 @@
       <c r="D266" t="n">
         <v>265</v>
       </c>
+      <c r="E266" t="n">
+        <v>265</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
@@ -4173,6 +4973,9 @@
       <c r="D267" t="n">
         <v>266</v>
       </c>
+      <c r="E267" t="n">
+        <v>266</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
@@ -4187,6 +4990,9 @@
       <c r="D268" t="n">
         <v>267</v>
       </c>
+      <c r="E268" t="n">
+        <v>267</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
@@ -4201,6 +5007,9 @@
       <c r="D269" t="n">
         <v>268</v>
       </c>
+      <c r="E269" t="n">
+        <v>268</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
@@ -4215,6 +5024,9 @@
       <c r="D270" t="n">
         <v>269</v>
       </c>
+      <c r="E270" t="n">
+        <v>269</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
@@ -4229,6 +5041,9 @@
       <c r="D271" t="n">
         <v>270</v>
       </c>
+      <c r="E271" t="n">
+        <v>270</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
@@ -4243,6 +5058,9 @@
       <c r="D272" t="n">
         <v>271</v>
       </c>
+      <c r="E272" t="n">
+        <v>271</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
@@ -4257,6 +5075,9 @@
       <c r="D273" t="n">
         <v>272</v>
       </c>
+      <c r="E273" t="n">
+        <v>272</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
@@ -4271,6 +5092,9 @@
       <c r="D274" t="n">
         <v>273</v>
       </c>
+      <c r="E274" t="n">
+        <v>273</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
@@ -4285,6 +5109,9 @@
       <c r="D275" t="n">
         <v>274</v>
       </c>
+      <c r="E275" t="n">
+        <v>274</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
@@ -4299,6 +5126,9 @@
       <c r="D276" t="n">
         <v>275</v>
       </c>
+      <c r="E276" t="n">
+        <v>275</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
@@ -4313,6 +5143,9 @@
       <c r="D277" t="n">
         <v>276</v>
       </c>
+      <c r="E277" t="n">
+        <v>276</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
@@ -4327,6 +5160,9 @@
       <c r="D278" t="n">
         <v>277</v>
       </c>
+      <c r="E278" t="n">
+        <v>277</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
@@ -4341,6 +5177,9 @@
       <c r="D279" t="n">
         <v>278</v>
       </c>
+      <c r="E279" t="n">
+        <v>278</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
@@ -4355,6 +5194,9 @@
       <c r="D280" t="n">
         <v>279</v>
       </c>
+      <c r="E280" t="n">
+        <v>279</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
@@ -4369,6 +5211,9 @@
       <c r="D281" t="n">
         <v>280</v>
       </c>
+      <c r="E281" t="n">
+        <v>280</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
@@ -4383,6 +5228,9 @@
       <c r="D282" t="n">
         <v>281</v>
       </c>
+      <c r="E282" t="n">
+        <v>281</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
@@ -4397,6 +5245,9 @@
       <c r="D283" t="n">
         <v>282</v>
       </c>
+      <c r="E283" t="n">
+        <v>282</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
@@ -4411,6 +5262,9 @@
       <c r="D284" t="n">
         <v>283</v>
       </c>
+      <c r="E284" t="n">
+        <v>283</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
@@ -4425,6 +5279,9 @@
       <c r="D285" t="n">
         <v>284</v>
       </c>
+      <c r="E285" t="n">
+        <v>284</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
@@ -4439,6 +5296,9 @@
       <c r="D286" t="n">
         <v>285</v>
       </c>
+      <c r="E286" t="n">
+        <v>285</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
@@ -4453,6 +5313,9 @@
       <c r="D287" t="n">
         <v>286</v>
       </c>
+      <c r="E287" t="n">
+        <v>286</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
@@ -4467,6 +5330,9 @@
       <c r="D288" t="n">
         <v>287</v>
       </c>
+      <c r="E288" t="n">
+        <v>287</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
@@ -4481,6 +5347,9 @@
       <c r="D289" t="n">
         <v>288</v>
       </c>
+      <c r="E289" t="n">
+        <v>288</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="n">
@@ -4495,6 +5364,9 @@
       <c r="D290" t="n">
         <v>289</v>
       </c>
+      <c r="E290" t="n">
+        <v>289</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="n">
@@ -4509,6 +5381,9 @@
       <c r="D291" t="n">
         <v>290</v>
       </c>
+      <c r="E291" t="n">
+        <v>290</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="n">
@@ -4523,6 +5398,9 @@
       <c r="D292" t="n">
         <v>291</v>
       </c>
+      <c r="E292" t="n">
+        <v>291</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
@@ -4537,6 +5415,9 @@
       <c r="D293" t="n">
         <v>292</v>
       </c>
+      <c r="E293" t="n">
+        <v>292</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="n">
@@ -4551,6 +5432,9 @@
       <c r="D294" t="n">
         <v>293</v>
       </c>
+      <c r="E294" t="n">
+        <v>293</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="n">
@@ -4565,6 +5449,9 @@
       <c r="D295" t="n">
         <v>294</v>
       </c>
+      <c r="E295" t="n">
+        <v>294</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="n">
@@ -4579,6 +5466,9 @@
       <c r="D296" t="n">
         <v>295</v>
       </c>
+      <c r="E296" t="n">
+        <v>295</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="n">
@@ -4593,6 +5483,9 @@
       <c r="D297" t="n">
         <v>296</v>
       </c>
+      <c r="E297" t="n">
+        <v>296</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="n">
@@ -4607,6 +5500,9 @@
       <c r="D298" t="n">
         <v>297</v>
       </c>
+      <c r="E298" t="n">
+        <v>297</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="n">
@@ -4621,6 +5517,9 @@
       <c r="D299" t="n">
         <v>298</v>
       </c>
+      <c r="E299" t="n">
+        <v>298</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
@@ -4635,6 +5534,9 @@
       <c r="D300" t="n">
         <v>299</v>
       </c>
+      <c r="E300" t="n">
+        <v>299</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="n">
@@ -4649,6 +5551,9 @@
       <c r="D301" t="n">
         <v>300</v>
       </c>
+      <c r="E301" t="n">
+        <v>300</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
@@ -4663,6 +5568,9 @@
       <c r="D302" t="n">
         <v>301</v>
       </c>
+      <c r="E302" t="n">
+        <v>301</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="n">
@@ -4677,6 +5585,9 @@
       <c r="D303" t="n">
         <v>302</v>
       </c>
+      <c r="E303" t="n">
+        <v>302</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="n">
@@ -4691,6 +5602,9 @@
       <c r="D304" t="n">
         <v>303</v>
       </c>
+      <c r="E304" t="n">
+        <v>303</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="n">
@@ -4705,6 +5619,9 @@
       <c r="D305" t="n">
         <v>304</v>
       </c>
+      <c r="E305" t="n">
+        <v>304</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
@@ -4719,6 +5636,9 @@
       <c r="D306" t="n">
         <v>305</v>
       </c>
+      <c r="E306" t="n">
+        <v>305</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="n">
@@ -4733,6 +5653,9 @@
       <c r="D307" t="n">
         <v>306</v>
       </c>
+      <c r="E307" t="n">
+        <v>306</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
@@ -4747,6 +5670,9 @@
       <c r="D308" t="n">
         <v>307</v>
       </c>
+      <c r="E308" t="n">
+        <v>307</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="n">
@@ -4761,6 +5687,9 @@
       <c r="D309" t="n">
         <v>308</v>
       </c>
+      <c r="E309" t="n">
+        <v>308</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="n">
@@ -4775,6 +5704,9 @@
       <c r="D310" t="n">
         <v>309</v>
       </c>
+      <c r="E310" t="n">
+        <v>309</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="n">
@@ -4789,6 +5721,9 @@
       <c r="D311" t="n">
         <v>310</v>
       </c>
+      <c r="E311" t="n">
+        <v>310</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="n">
@@ -4803,6 +5738,9 @@
       <c r="D312" t="n">
         <v>311</v>
       </c>
+      <c r="E312" t="n">
+        <v>311</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="n">
@@ -4817,6 +5755,9 @@
       <c r="D313" t="n">
         <v>312</v>
       </c>
+      <c r="E313" t="n">
+        <v>312</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="n">
@@ -4831,6 +5772,9 @@
       <c r="D314" t="n">
         <v>313</v>
       </c>
+      <c r="E314" t="n">
+        <v>313</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="n">
@@ -4845,6 +5789,9 @@
       <c r="D315" t="n">
         <v>314</v>
       </c>
+      <c r="E315" t="n">
+        <v>314</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="n">
@@ -4859,6 +5806,9 @@
       <c r="D316" t="n">
         <v>315</v>
       </c>
+      <c r="E316" t="n">
+        <v>315</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="n">
@@ -4873,6 +5823,9 @@
       <c r="D317" t="n">
         <v>316</v>
       </c>
+      <c r="E317" t="n">
+        <v>316</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="n">
@@ -4887,6 +5840,9 @@
       <c r="D318" t="n">
         <v>317</v>
       </c>
+      <c r="E318" t="n">
+        <v>317</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
@@ -4901,6 +5857,9 @@
       <c r="D319" t="n">
         <v>318</v>
       </c>
+      <c r="E319" t="n">
+        <v>318</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="n">
@@ -4915,6 +5874,9 @@
       <c r="D320" t="n">
         <v>319</v>
       </c>
+      <c r="E320" t="n">
+        <v>319</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="n">
@@ -4929,6 +5891,9 @@
       <c r="D321" t="n">
         <v>320</v>
       </c>
+      <c r="E321" t="n">
+        <v>320</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="n">
@@ -4943,6 +5908,9 @@
       <c r="D322" t="n">
         <v>321</v>
       </c>
+      <c r="E322" t="n">
+        <v>321</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="n">
@@ -4957,6 +5925,9 @@
       <c r="D323" t="n">
         <v>322</v>
       </c>
+      <c r="E323" t="n">
+        <v>322</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="n">
@@ -4971,6 +5942,9 @@
       <c r="D324" t="n">
         <v>323</v>
       </c>
+      <c r="E324" t="n">
+        <v>323</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="n">
@@ -4985,6 +5959,9 @@
       <c r="D325" t="n">
         <v>324</v>
       </c>
+      <c r="E325" t="n">
+        <v>324</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="n">
@@ -4999,6 +5976,9 @@
       <c r="D326" t="n">
         <v>325</v>
       </c>
+      <c r="E326" t="n">
+        <v>325</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="n">
@@ -5013,6 +5993,9 @@
       <c r="D327" t="n">
         <v>326</v>
       </c>
+      <c r="E327" t="n">
+        <v>326</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="n">
@@ -5027,6 +6010,9 @@
       <c r="D328" t="n">
         <v>327</v>
       </c>
+      <c r="E328" t="n">
+        <v>327</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
@@ -5041,6 +6027,9 @@
       <c r="D329" t="n">
         <v>328</v>
       </c>
+      <c r="E329" t="n">
+        <v>328</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="n">
@@ -5055,6 +6044,9 @@
       <c r="D330" t="n">
         <v>329</v>
       </c>
+      <c r="E330" t="n">
+        <v>329</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
@@ -5069,6 +6061,9 @@
       <c r="D331" t="n">
         <v>330</v>
       </c>
+      <c r="E331" t="n">
+        <v>330</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" s="1" t="n">
@@ -5083,6 +6078,9 @@
       <c r="D332" t="n">
         <v>331</v>
       </c>
+      <c r="E332" t="n">
+        <v>331</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" s="1" t="n">
@@ -5097,6 +6095,9 @@
       <c r="D333" t="n">
         <v>332</v>
       </c>
+      <c r="E333" t="n">
+        <v>332</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
@@ -5111,6 +6112,9 @@
       <c r="D334" t="n">
         <v>333</v>
       </c>
+      <c r="E334" t="n">
+        <v>333</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" s="1" t="n">
@@ -5125,6 +6129,9 @@
       <c r="D335" t="n">
         <v>334</v>
       </c>
+      <c r="E335" t="n">
+        <v>334</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" s="1" t="n">
@@ -5139,6 +6146,9 @@
       <c r="D336" t="n">
         <v>335</v>
       </c>
+      <c r="E336" t="n">
+        <v>335</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" s="1" t="n">
@@ -5153,6 +6163,9 @@
       <c r="D337" t="n">
         <v>336</v>
       </c>
+      <c r="E337" t="n">
+        <v>336</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="n">
@@ -5167,6 +6180,9 @@
       <c r="D338" t="n">
         <v>337</v>
       </c>
+      <c r="E338" t="n">
+        <v>337</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" s="1" t="n">
@@ -5181,6 +6197,9 @@
       <c r="D339" t="n">
         <v>338</v>
       </c>
+      <c r="E339" t="n">
+        <v>338</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
@@ -5195,6 +6214,9 @@
       <c r="D340" t="n">
         <v>339</v>
       </c>
+      <c r="E340" t="n">
+        <v>339</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
@@ -5209,6 +6231,9 @@
       <c r="D341" t="n">
         <v>340</v>
       </c>
+      <c r="E341" t="n">
+        <v>340</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
@@ -5223,6 +6248,9 @@
       <c r="D342" t="n">
         <v>341</v>
       </c>
+      <c r="E342" t="n">
+        <v>341</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" s="1" t="n">
@@ -5237,6 +6265,9 @@
       <c r="D343" t="n">
         <v>342</v>
       </c>
+      <c r="E343" t="n">
+        <v>342</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" s="1" t="n">
@@ -5251,6 +6282,9 @@
       <c r="D344" t="n">
         <v>343</v>
       </c>
+      <c r="E344" t="n">
+        <v>343</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" s="1" t="n">
@@ -5265,6 +6299,9 @@
       <c r="D345" t="n">
         <v>344</v>
       </c>
+      <c r="E345" t="n">
+        <v>344</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" s="1" t="n">
@@ -5279,6 +6316,9 @@
       <c r="D346" t="n">
         <v>345</v>
       </c>
+      <c r="E346" t="n">
+        <v>345</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" s="1" t="n">
@@ -5293,6 +6333,9 @@
       <c r="D347" t="n">
         <v>346</v>
       </c>
+      <c r="E347" t="n">
+        <v>346</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" s="1" t="n">
@@ -5307,6 +6350,9 @@
       <c r="D348" t="n">
         <v>347</v>
       </c>
+      <c r="E348" t="n">
+        <v>347</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
@@ -5321,6 +6367,9 @@
       <c r="D349" t="n">
         <v>348</v>
       </c>
+      <c r="E349" t="n">
+        <v>348</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" s="1" t="n">
@@ -5335,6 +6384,9 @@
       <c r="D350" t="n">
         <v>349</v>
       </c>
+      <c r="E350" t="n">
+        <v>349</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" s="1" t="n">
@@ -5349,6 +6401,9 @@
       <c r="D351" t="n">
         <v>350</v>
       </c>
+      <c r="E351" t="n">
+        <v>350</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" s="1" t="n">
@@ -5363,6 +6418,9 @@
       <c r="D352" t="n">
         <v>351</v>
       </c>
+      <c r="E352" t="n">
+        <v>351</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" s="1" t="n">
@@ -5377,6 +6435,9 @@
       <c r="D353" t="n">
         <v>352</v>
       </c>
+      <c r="E353" t="n">
+        <v>352</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" s="1" t="n">
@@ -5391,6 +6452,9 @@
       <c r="D354" t="n">
         <v>353</v>
       </c>
+      <c r="E354" t="n">
+        <v>353</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" s="1" t="n">
@@ -5405,6 +6469,9 @@
       <c r="D355" t="n">
         <v>354</v>
       </c>
+      <c r="E355" t="n">
+        <v>354</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" s="1" t="n">
@@ -5419,6 +6486,9 @@
       <c r="D356" t="n">
         <v>355</v>
       </c>
+      <c r="E356" t="n">
+        <v>355</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" s="1" t="n">
@@ -5433,6 +6503,9 @@
       <c r="D357" t="n">
         <v>356</v>
       </c>
+      <c r="E357" t="n">
+        <v>356</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358" s="1" t="n">
@@ -5447,6 +6520,9 @@
       <c r="D358" t="n">
         <v>357</v>
       </c>
+      <c r="E358" t="n">
+        <v>357</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" s="1" t="n">
@@ -5461,6 +6537,9 @@
       <c r="D359" t="n">
         <v>358</v>
       </c>
+      <c r="E359" t="n">
+        <v>358</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360" s="1" t="n">
@@ -5475,6 +6554,9 @@
       <c r="D360" t="n">
         <v>359</v>
       </c>
+      <c r="E360" t="n">
+        <v>359</v>
+      </c>
     </row>
     <row r="361">
       <c r="A361" s="1" t="n">
@@ -5489,6 +6571,9 @@
       <c r="D361" t="n">
         <v>360</v>
       </c>
+      <c r="E361" t="n">
+        <v>360</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362" s="1" t="n">
@@ -5503,6 +6588,9 @@
       <c r="D362" t="n">
         <v>361</v>
       </c>
+      <c r="E362" t="n">
+        <v>361</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363" s="1" t="n">
@@ -5517,6 +6605,9 @@
       <c r="D363" t="n">
         <v>362</v>
       </c>
+      <c r="E363" t="n">
+        <v>362</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364" s="1" t="n">
@@ -5531,6 +6622,9 @@
       <c r="D364" t="n">
         <v>363</v>
       </c>
+      <c r="E364" t="n">
+        <v>363</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" s="1" t="n">
@@ -5545,6 +6639,9 @@
       <c r="D365" t="n">
         <v>364</v>
       </c>
+      <c r="E365" t="n">
+        <v>364</v>
+      </c>
     </row>
     <row r="366">
       <c r="A366" s="1" t="n">
@@ -5559,6 +6656,9 @@
       <c r="D366" t="n">
         <v>365</v>
       </c>
+      <c r="E366" t="n">
+        <v>365</v>
+      </c>
     </row>
     <row r="367">
       <c r="A367" s="1" t="n">
@@ -5573,6 +6673,9 @@
       <c r="D367" t="n">
         <v>366</v>
       </c>
+      <c r="E367" t="n">
+        <v>366</v>
+      </c>
     </row>
     <row r="368">
       <c r="A368" s="1" t="n">
@@ -5587,6 +6690,9 @@
       <c r="D368" t="n">
         <v>367</v>
       </c>
+      <c r="E368" t="n">
+        <v>367</v>
+      </c>
     </row>
     <row r="369">
       <c r="A369" s="1" t="n">
@@ -5601,6 +6707,9 @@
       <c r="D369" t="n">
         <v>368</v>
       </c>
+      <c r="E369" t="n">
+        <v>368</v>
+      </c>
     </row>
     <row r="370">
       <c r="A370" s="1" t="n">
@@ -5615,6 +6724,9 @@
       <c r="D370" t="n">
         <v>369</v>
       </c>
+      <c r="E370" t="n">
+        <v>369</v>
+      </c>
     </row>
     <row r="371">
       <c r="A371" s="1" t="n">
@@ -5629,6 +6741,9 @@
       <c r="D371" t="n">
         <v>370</v>
       </c>
+      <c r="E371" t="n">
+        <v>370</v>
+      </c>
     </row>
     <row r="372">
       <c r="A372" s="1" t="n">
@@ -5643,6 +6758,9 @@
       <c r="D372" t="n">
         <v>371</v>
       </c>
+      <c r="E372" t="n">
+        <v>371</v>
+      </c>
     </row>
     <row r="373">
       <c r="A373" s="1" t="n">
@@ -5657,6 +6775,9 @@
       <c r="D373" t="n">
         <v>372</v>
       </c>
+      <c r="E373" t="n">
+        <v>372</v>
+      </c>
     </row>
     <row r="374">
       <c r="A374" s="1" t="n">
@@ -5671,6 +6792,9 @@
       <c r="D374" t="n">
         <v>373</v>
       </c>
+      <c r="E374" t="n">
+        <v>373</v>
+      </c>
     </row>
     <row r="375">
       <c r="A375" s="1" t="n">
@@ -5685,6 +6809,9 @@
       <c r="D375" t="n">
         <v>374</v>
       </c>
+      <c r="E375" t="n">
+        <v>374</v>
+      </c>
     </row>
     <row r="376">
       <c r="A376" s="1" t="n">
@@ -5699,6 +6826,9 @@
       <c r="D376" t="n">
         <v>375</v>
       </c>
+      <c r="E376" t="n">
+        <v>375</v>
+      </c>
     </row>
     <row r="377">
       <c r="A377" s="1" t="n">
@@ -5713,6 +6843,9 @@
       <c r="D377" t="n">
         <v>376</v>
       </c>
+      <c r="E377" t="n">
+        <v>376</v>
+      </c>
     </row>
     <row r="378">
       <c r="A378" s="1" t="n">
@@ -5727,6 +6860,9 @@
       <c r="D378" t="n">
         <v>377</v>
       </c>
+      <c r="E378" t="n">
+        <v>377</v>
+      </c>
     </row>
     <row r="379">
       <c r="A379" s="1" t="n">
@@ -5741,6 +6877,9 @@
       <c r="D379" t="n">
         <v>378</v>
       </c>
+      <c r="E379" t="n">
+        <v>378</v>
+      </c>
     </row>
     <row r="380">
       <c r="A380" s="1" t="n">
@@ -5755,6 +6894,9 @@
       <c r="D380" t="n">
         <v>379</v>
       </c>
+      <c r="E380" t="n">
+        <v>379</v>
+      </c>
     </row>
     <row r="381">
       <c r="A381" s="1" t="n">
@@ -5769,6 +6911,9 @@
       <c r="D381" t="n">
         <v>380</v>
       </c>
+      <c r="E381" t="n">
+        <v>380</v>
+      </c>
     </row>
     <row r="382">
       <c r="A382" s="1" t="n">
@@ -5783,6 +6928,9 @@
       <c r="D382" t="n">
         <v>381</v>
       </c>
+      <c r="E382" t="n">
+        <v>381</v>
+      </c>
     </row>
     <row r="383">
       <c r="A383" s="1" t="n">
@@ -5797,6 +6945,9 @@
       <c r="D383" t="n">
         <v>382</v>
       </c>
+      <c r="E383" t="n">
+        <v>382</v>
+      </c>
     </row>
     <row r="384">
       <c r="A384" s="1" t="n">
@@ -5811,6 +6962,9 @@
       <c r="D384" t="n">
         <v>383</v>
       </c>
+      <c r="E384" t="n">
+        <v>383</v>
+      </c>
     </row>
     <row r="385">
       <c r="A385" s="1" t="n">
@@ -5825,6 +6979,9 @@
       <c r="D385" t="n">
         <v>384</v>
       </c>
+      <c r="E385" t="n">
+        <v>384</v>
+      </c>
     </row>
     <row r="386">
       <c r="A386" s="1" t="n">
@@ -5839,6 +6996,9 @@
       <c r="D386" t="n">
         <v>385</v>
       </c>
+      <c r="E386" t="n">
+        <v>385</v>
+      </c>
     </row>
     <row r="387">
       <c r="A387" s="1" t="n">
@@ -5853,6 +7013,9 @@
       <c r="D387" t="n">
         <v>386</v>
       </c>
+      <c r="E387" t="n">
+        <v>386</v>
+      </c>
     </row>
     <row r="388">
       <c r="A388" s="1" t="n">
@@ -5867,6 +7030,9 @@
       <c r="D388" t="n">
         <v>387</v>
       </c>
+      <c r="E388" t="n">
+        <v>387</v>
+      </c>
     </row>
     <row r="389">
       <c r="A389" s="1" t="n">
@@ -5881,6 +7047,9 @@
       <c r="D389" t="n">
         <v>388</v>
       </c>
+      <c r="E389" t="n">
+        <v>388</v>
+      </c>
     </row>
     <row r="390">
       <c r="A390" s="1" t="n">
@@ -5895,6 +7064,9 @@
       <c r="D390" t="n">
         <v>389</v>
       </c>
+      <c r="E390" t="n">
+        <v>389</v>
+      </c>
     </row>
     <row r="391">
       <c r="A391" s="1" t="n">
@@ -5909,6 +7081,9 @@
       <c r="D391" t="n">
         <v>390</v>
       </c>
+      <c r="E391" t="n">
+        <v>390</v>
+      </c>
     </row>
     <row r="392">
       <c r="A392" s="1" t="n">
@@ -5923,6 +7098,9 @@
       <c r="D392" t="n">
         <v>391</v>
       </c>
+      <c r="E392" t="n">
+        <v>391</v>
+      </c>
     </row>
     <row r="393">
       <c r="A393" s="1" t="n">
@@ -5937,6 +7115,9 @@
       <c r="D393" t="n">
         <v>392</v>
       </c>
+      <c r="E393" t="n">
+        <v>392</v>
+      </c>
     </row>
     <row r="394">
       <c r="A394" s="1" t="n">
@@ -5951,6 +7132,9 @@
       <c r="D394" t="n">
         <v>393</v>
       </c>
+      <c r="E394" t="n">
+        <v>393</v>
+      </c>
     </row>
     <row r="395">
       <c r="A395" s="1" t="n">
@@ -5965,6 +7149,9 @@
       <c r="D395" t="n">
         <v>394</v>
       </c>
+      <c r="E395" t="n">
+        <v>394</v>
+      </c>
     </row>
     <row r="396">
       <c r="A396" s="1" t="n">
@@ -5979,6 +7166,9 @@
       <c r="D396" t="n">
         <v>395</v>
       </c>
+      <c r="E396" t="n">
+        <v>395</v>
+      </c>
     </row>
     <row r="397">
       <c r="A397" s="1" t="n">
@@ -5993,6 +7183,9 @@
       <c r="D397" t="n">
         <v>396</v>
       </c>
+      <c r="E397" t="n">
+        <v>396</v>
+      </c>
     </row>
     <row r="398">
       <c r="A398" s="1" t="n">
@@ -6007,6 +7200,9 @@
       <c r="D398" t="n">
         <v>397</v>
       </c>
+      <c r="E398" t="n">
+        <v>397</v>
+      </c>
     </row>
     <row r="399">
       <c r="A399" s="1" t="n">
@@ -6021,6 +7217,9 @@
       <c r="D399" t="n">
         <v>398</v>
       </c>
+      <c r="E399" t="n">
+        <v>398</v>
+      </c>
     </row>
     <row r="400">
       <c r="A400" s="1" t="n">
@@ -6035,6 +7234,9 @@
       <c r="D400" t="n">
         <v>399</v>
       </c>
+      <c r="E400" t="n">
+        <v>399</v>
+      </c>
     </row>
     <row r="401">
       <c r="A401" s="1" t="n">
@@ -6049,6 +7251,9 @@
       <c r="D401" t="n">
         <v>400</v>
       </c>
+      <c r="E401" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="402">
       <c r="A402" s="1" t="n">
@@ -6063,6 +7268,9 @@
       <c r="D402" t="n">
         <v>401</v>
       </c>
+      <c r="E402" t="n">
+        <v>401</v>
+      </c>
     </row>
     <row r="403">
       <c r="A403" s="1" t="n">
@@ -6077,6 +7285,9 @@
       <c r="D403" t="n">
         <v>402</v>
       </c>
+      <c r="E403" t="n">
+        <v>402</v>
+      </c>
     </row>
     <row r="404">
       <c r="A404" s="1" t="n">
@@ -6091,6 +7302,9 @@
       <c r="D404" t="n">
         <v>403</v>
       </c>
+      <c r="E404" t="n">
+        <v>403</v>
+      </c>
     </row>
     <row r="405">
       <c r="A405" s="1" t="n">
@@ -6105,6 +7319,9 @@
       <c r="D405" t="n">
         <v>404</v>
       </c>
+      <c r="E405" t="n">
+        <v>404</v>
+      </c>
     </row>
     <row r="406">
       <c r="A406" s="1" t="n">
@@ -6119,6 +7336,9 @@
       <c r="D406" t="n">
         <v>405</v>
       </c>
+      <c r="E406" t="n">
+        <v>405</v>
+      </c>
     </row>
     <row r="407">
       <c r="A407" s="1" t="n">
@@ -6133,6 +7353,9 @@
       <c r="D407" t="n">
         <v>406</v>
       </c>
+      <c r="E407" t="n">
+        <v>406</v>
+      </c>
     </row>
     <row r="408">
       <c r="A408" s="1" t="n">
@@ -6147,6 +7370,9 @@
       <c r="D408" t="n">
         <v>407</v>
       </c>
+      <c r="E408" t="n">
+        <v>407</v>
+      </c>
     </row>
     <row r="409">
       <c r="A409" s="1" t="n">
@@ -6161,6 +7387,9 @@
       <c r="D409" t="n">
         <v>408</v>
       </c>
+      <c r="E409" t="n">
+        <v>408</v>
+      </c>
     </row>
     <row r="410">
       <c r="A410" s="1" t="n">
@@ -6175,6 +7404,9 @@
       <c r="D410" t="n">
         <v>409</v>
       </c>
+      <c r="E410" t="n">
+        <v>409</v>
+      </c>
     </row>
     <row r="411">
       <c r="A411" s="1" t="n">
@@ -6189,6 +7421,9 @@
       <c r="D411" t="n">
         <v>410</v>
       </c>
+      <c r="E411" t="n">
+        <v>410</v>
+      </c>
     </row>
     <row r="412">
       <c r="A412" s="1" t="n">
@@ -6203,6 +7438,9 @@
       <c r="D412" t="n">
         <v>411</v>
       </c>
+      <c r="E412" t="n">
+        <v>411</v>
+      </c>
     </row>
     <row r="413">
       <c r="A413" s="1" t="n">
@@ -6217,6 +7455,9 @@
       <c r="D413" t="n">
         <v>412</v>
       </c>
+      <c r="E413" t="n">
+        <v>412</v>
+      </c>
     </row>
     <row r="414">
       <c r="A414" s="1" t="n">
@@ -6231,6 +7472,9 @@
       <c r="D414" t="n">
         <v>413</v>
       </c>
+      <c r="E414" t="n">
+        <v>413</v>
+      </c>
     </row>
     <row r="415">
       <c r="A415" s="1" t="n">
@@ -6245,6 +7489,9 @@
       <c r="D415" t="n">
         <v>414</v>
       </c>
+      <c r="E415" t="n">
+        <v>414</v>
+      </c>
     </row>
     <row r="416">
       <c r="A416" s="1" t="n">
@@ -6259,6 +7506,9 @@
       <c r="D416" t="n">
         <v>415</v>
       </c>
+      <c r="E416" t="n">
+        <v>415</v>
+      </c>
     </row>
     <row r="417">
       <c r="A417" s="1" t="n">
@@ -6273,6 +7523,9 @@
       <c r="D417" t="n">
         <v>416</v>
       </c>
+      <c r="E417" t="n">
+        <v>416</v>
+      </c>
     </row>
     <row r="418">
       <c r="A418" s="1" t="n">
@@ -6287,6 +7540,9 @@
       <c r="D418" t="n">
         <v>417</v>
       </c>
+      <c r="E418" t="n">
+        <v>417</v>
+      </c>
     </row>
     <row r="419">
       <c r="A419" s="1" t="n">
@@ -6301,6 +7557,9 @@
       <c r="D419" t="n">
         <v>418</v>
       </c>
+      <c r="E419" t="n">
+        <v>418</v>
+      </c>
     </row>
     <row r="420">
       <c r="A420" s="1" t="n">
@@ -6315,6 +7574,9 @@
       <c r="D420" t="n">
         <v>419</v>
       </c>
+      <c r="E420" t="n">
+        <v>419</v>
+      </c>
     </row>
     <row r="421">
       <c r="A421" s="1" t="n">
@@ -6329,6 +7591,9 @@
       <c r="D421" t="n">
         <v>420</v>
       </c>
+      <c r="E421" t="n">
+        <v>420</v>
+      </c>
     </row>
     <row r="422">
       <c r="A422" s="1" t="n">
@@ -6343,6 +7608,9 @@
       <c r="D422" t="n">
         <v>421</v>
       </c>
+      <c r="E422" t="n">
+        <v>421</v>
+      </c>
     </row>
     <row r="423">
       <c r="A423" s="1" t="n">
@@ -6357,6 +7625,9 @@
       <c r="D423" t="n">
         <v>422</v>
       </c>
+      <c r="E423" t="n">
+        <v>422</v>
+      </c>
     </row>
     <row r="424">
       <c r="A424" s="1" t="n">
@@ -6371,6 +7642,9 @@
       <c r="D424" t="n">
         <v>423</v>
       </c>
+      <c r="E424" t="n">
+        <v>423</v>
+      </c>
     </row>
     <row r="425">
       <c r="A425" s="1" t="n">
@@ -6385,6 +7659,9 @@
       <c r="D425" t="n">
         <v>424</v>
       </c>
+      <c r="E425" t="n">
+        <v>424</v>
+      </c>
     </row>
     <row r="426">
       <c r="A426" s="1" t="n">
@@ -6399,6 +7676,9 @@
       <c r="D426" t="n">
         <v>425</v>
       </c>
+      <c r="E426" t="n">
+        <v>425</v>
+      </c>
     </row>
     <row r="427">
       <c r="A427" s="1" t="n">
@@ -6411,6 +7691,9 @@
         <v>4</v>
       </c>
       <c r="D427" t="n">
+        <v>426</v>
+      </c>
+      <c r="E427" t="n">
         <v>426</v>
       </c>
     </row>

</xml_diff>